<commit_message>
Commit with the Corporate User Back-End code without the dynamic URL part
</commit_message>
<xml_diff>
--- a/media/uploads/Indiv_hitesh25_Data.xlsx
+++ b/media/uploads/Indiv_hitesh25_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="budget" sheetId="1" state="visible" r:id="rId1"/>
@@ -386,10 +386,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -434,10 +434,10 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="n">
-        <v>10000</v>
+        <v>35000</v>
       </c>
       <c r="B2" t="n">
-        <v>20000</v>
+        <v>15000</v>
       </c>
       <c r="C2" t="n">
         <v>12000</v>
@@ -468,6 +468,424 @@
       </c>
       <c r="L2" t="n">
         <v>200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K3" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I4" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J4" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K4" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I5" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J5" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="n">
+        <v>15000</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I6" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J6" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K6" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L6" t="n">
+        <v>185000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I7" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K7" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I8" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K8" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L8" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H9" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I9" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J9" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K9" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L9" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I10" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K10" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L10" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I11" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J11" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K11" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I12" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K12" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L12" t="n">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>15000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I13" t="n">
+        <v>45000</v>
+      </c>
+      <c r="J13" t="n">
+        <v>30000</v>
+      </c>
+      <c r="K13" t="n">
+        <v>15000</v>
+      </c>
+      <c r="L13" t="n">
+        <v>180000</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +947,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="n">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="B2" t="n">
         <v>3500</v>
@@ -562,12 +980,12 @@
         <v>15000</v>
       </c>
       <c r="L2" t="n">
-        <v>126000</v>
+        <v>128000</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="n">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="B3" t="n">
         <v>7000</v>
@@ -600,12 +1018,12 @@
         <v>15000</v>
       </c>
       <c r="L3" t="n">
-        <v>146000</v>
+        <v>151000</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="n">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="B4" t="n">
         <v>8000</v>
@@ -638,7 +1056,7 @@
         <v>15000</v>
       </c>
       <c r="L4" t="n">
-        <v>142600</v>
+        <v>147600</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -681,7 +1099,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="n">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="B6" t="n">
         <v>5000</v>
@@ -714,7 +1132,7 @@
         <v>15000</v>
       </c>
       <c r="L6" t="n">
-        <v>127550</v>
+        <v>132550</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -833,7 +1251,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="n">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="B10" t="n">
         <v>14000</v>
@@ -866,7 +1284,7 @@
         <v>15000</v>
       </c>
       <c r="L10" t="n">
-        <v>156821</v>
+        <v>158821</v>
       </c>
     </row>
     <row r="11" spans="1:12">

</xml_diff>

<commit_message>
Commit with all major chunks of the code completed with design yet left to be integrated.
</commit_message>
<xml_diff>
--- a/media/uploads/Indiv_hitesh25_Data.xlsx
+++ b/media/uploads/Indiv_hitesh25_Data.xlsx
@@ -434,7 +434,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="n">
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="B2" t="n">
         <v>15000</v>
@@ -467,7 +467,7 @@
         <v>15000</v>
       </c>
       <c r="L2" t="n">
-        <v>200000</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="3" spans="1:12">

</xml_diff>